<commit_message>
more refactoring of ipdc_dashboard code
</commit_message>
<xml_diff>
--- a/tests/resources/benefits_master_test_1_2020.xlsx
+++ b/tests/resources/benefits_master_test_1_2020.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="303">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -902,6 +902,33 @@
   </si>
   <si>
     <t xml:space="preserve">No deductions - Calc Net BEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project stage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adjusted Benefits Cost Ratio (BCR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial Benefits Cost Ratio (BCR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VfM Category single entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VfM Category lower range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VfM Category upper range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRO Benefits RAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red</t>
   </si>
 </sst>
 </file>
@@ -1076,8 +1103,8 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A262" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A270" activeCellId="0" sqref="A270"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A272" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A291" activeCellId="0" sqref="A291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4967,13 +4994,59 @@
         <v>292</v>
       </c>
     </row>
-    <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A284" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A285" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B285" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="C285" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="D285" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A286" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A287" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A288" s="0" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A289" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A290" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="B290" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="C290" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="D290" s="0" t="s">
+        <v>301</v>
+      </c>
+    </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
all tests passing apart from test_data_queries_milestones
</commit_message>
<xml_diff>
--- a/tests/resources/benefits_master_test_1_2020.xlsx
+++ b/tests/resources/benefits_master_test_1_2020.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="304">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -929,6 +929,9 @@
   </si>
   <si>
     <t xml:space="preserve">Red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GMPP - IPA ID Number</t>
   </si>
 </sst>
 </file>
@@ -5047,7 +5050,11 @@
         <v>301</v>
       </c>
     </row>
-    <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="0" t="s">
+        <v>303</v>
+      </c>
+    </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>